<commit_message>
one peptide had a space after
</commit_message>
<xml_diff>
--- a/data/TNF-alphaGN.xlsx
+++ b/data/TNF-alphaGN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raqie\Desktop\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasho\Documents\GitHub\coADAPTr\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B738BF-D1BF-4DD4-9BF4-24216D784CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A81DC0A-9CF0-4CDB-9BBB-3CA03EFEC7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="2" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AH$193</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="313">
   <si>
     <t>Checked</t>
   </si>
@@ -972,6 +975,9 @@
   </si>
   <si>
     <t>YLIYSQVLFKGQGCPSTHVLLTHTIS</t>
+  </si>
+  <si>
+    <t>TTLFCLLHFGVIGPQREEFPR</t>
   </si>
 </sst>
 </file>
@@ -1165,9 +1171,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1205,7 +1211,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1311,7 +1317,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1453,7 +1459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1466,8 +1472,8 @@
   </sheetPr>
   <dimension ref="A1:AH193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1801,7 +1807,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="2">
@@ -2617,7 +2623,7 @@
         <v>35</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="2">
@@ -3433,7 +3439,7 @@
         <v>35</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="2">
@@ -4253,7 +4259,7 @@
         <v>35</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>79</v>
@@ -5085,7 +5091,7 @@
         <v>35</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>79</v>
@@ -5917,7 +5923,7 @@
         <v>35</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>79</v>
@@ -6749,7 +6755,7 @@
         <v>35</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>86</v>
@@ -7581,7 +7587,7 @@
         <v>35</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>86</v>
@@ -8413,7 +8419,7 @@
         <v>35</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>86</v>
@@ -9245,7 +9251,7 @@
         <v>35</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>87</v>
@@ -10077,7 +10083,7 @@
         <v>35</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>87</v>
@@ -10909,7 +10915,7 @@
         <v>35</v>
       </c>
       <c r="E92" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>87</v>
@@ -11737,7 +11743,7 @@
         <v>35</v>
       </c>
       <c r="E100" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F100" s="6"/>
       <c r="G100" s="2">
@@ -12553,7 +12559,7 @@
         <v>35</v>
       </c>
       <c r="E108" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="2">
@@ -13369,7 +13375,7 @@
         <v>35</v>
       </c>
       <c r="E116" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F116" s="6"/>
       <c r="G116" s="2">
@@ -14189,7 +14195,7 @@
         <v>35</v>
       </c>
       <c r="E124" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F124" s="6" t="s">
         <v>79</v>
@@ -15021,7 +15027,7 @@
         <v>35</v>
       </c>
       <c r="E132" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F132" s="6" t="s">
         <v>79</v>
@@ -15853,7 +15859,7 @@
         <v>35</v>
       </c>
       <c r="E140" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F140" s="6" t="s">
         <v>79</v>
@@ -16685,7 +16691,7 @@
         <v>35</v>
       </c>
       <c r="E148" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F148" s="6" t="s">
         <v>86</v>
@@ -17517,7 +17523,7 @@
         <v>35</v>
       </c>
       <c r="E156" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F156" s="6" t="s">
         <v>86</v>
@@ -18349,7 +18355,7 @@
         <v>35</v>
       </c>
       <c r="E164" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F164" s="6" t="s">
         <v>86</v>
@@ -19181,7 +19187,7 @@
         <v>35</v>
       </c>
       <c r="E172" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F172" s="6" t="s">
         <v>87</v>
@@ -20013,7 +20019,7 @@
         <v>35</v>
       </c>
       <c r="E180" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F180" s="6" t="s">
         <v>87</v>
@@ -20845,7 +20851,7 @@
         <v>35</v>
       </c>
       <c r="E188" s="15" t="s">
-        <v>65</v>
+        <v>312</v>
       </c>
       <c r="F188" s="6" t="s">
         <v>87</v>

</xml_diff>